<commit_message>
Update macrophage annotation labels
</commit_message>
<xml_diff>
--- a/data/cluster_annotations/macrophages_26.06.24.xlsx
+++ b/data/cluster_annotations/macrophages_26.06.24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maksimovicjovana/Work/Projects/MCRI/melanie.neeland/paed-inflammation-CITEseq/data/cluster_annotations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petermacvic-my.sharepoint.com/personal/jovana_maksimovic_petermac_org/Documents/Work/Projects/MCRI/melanie.neeland/paed-inflammation-CITEseq/data/cluster_annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625DD4E9-C93A-FF42-A679-FCBFD6FA43BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{625DD4E9-C93A-FF42-A679-FCBFD6FA43BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{266421A8-FF4E-E64A-8023-9E16F5BF468C}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2940" windowWidth="29480" windowHeight="15900" xr2:uid="{6FB58300-E802-447C-A097-CCD1BBD9175D}"/>
+    <workbookView xWindow="33560" yWindow="3200" windowWidth="29480" windowHeight="15900" xr2:uid="{6FB58300-E802-447C-A097-CCD1BBD9175D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>Cluster</t>
   </si>
   <si>
-    <t>Annotation</t>
-  </si>
-  <si>
     <t>Relevant marker genes</t>
   </si>
   <si>
@@ -200,13 +197,22 @@
     <t>macro-proliferating-G2M</t>
   </si>
   <si>
-    <t>Broad</t>
-  </si>
-  <si>
-    <t>Macrophages</t>
-  </si>
-  <si>
-    <t>Proliferating macrophages</t>
+    <t>ann_level_1</t>
+  </si>
+  <si>
+    <t>ann_level_2</t>
+  </si>
+  <si>
+    <t>ann_level_3</t>
+  </si>
+  <si>
+    <t>macrophages</t>
+  </si>
+  <si>
+    <t>proliferating macrophages</t>
+  </si>
+  <si>
+    <t>macro-proliferating</t>
   </si>
 </sst>
 </file>
@@ -284,6 +290,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,376 +593,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC0FAB-9B9B-4D5C-BBD2-66DD99CDB8A0}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="5" width="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="6" width="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>35</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s">
+      <c r="G18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>